<commit_message>
Combining data quality measurement with data model quality.
</commit_message>
<xml_diff>
--- a/scheme/Conta_corrente/issues_metadados_conta_corrente.xlsx
+++ b/scheme/Conta_corrente/issues_metadados_conta_corrente.xlsx
@@ -8,10 +8,10 @@
   </bookViews>
   <sheets>
     <sheet name="0_SCHEMA_METADATA" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="1_ISSUES" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="2_SCHEME_MEASURES" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="3_MODEL_MEASURES" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="4_MODEL_METRICS" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="SCHEME_MEASURES" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="METADATA_ISSUES" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="METADATA_MEASURES" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="METADATA_METRICS" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14019,7 +14019,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14030,1754 +14030,94 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>rule</t>
+          <t>Indicator</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>desc</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>table</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>column</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>constraint_name</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>length</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>limit</t>
+          <t>Value</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MQMD06</t>
+          <t>MQMS01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Total number of tables with plural names</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>AUDITORIA_ENTIDADES</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+          <t>Total number of tables</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MQMD10</t>
+          <t>MQMS02</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>DEBITO_20180115</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>SEQ_DEBITO</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+          <t>Total number of columns</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>217</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MQMD10</t>
+          <t>MQMS03</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>DEBITO_20180115</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>SEQ_DEBITO_ORIGEM</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+          <t>Total number of primary key</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MQMD10</t>
+          <t>MQMS04</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>DEBITO_20180115</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>COD_RECEITA</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+          <t>Total number of foreign key</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MQMD10</t>
+          <t>MQMS05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>DEBITO_20180115</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>COD_INDICADOR</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>DEBITO_20180115</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>COD_PRODUTO_SERVICO</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>DEBITO_20180115</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>SEQ_PESSOA</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>DEBITO_20180115</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>DAT_VENCIMENTO</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>DEBITO_20180115</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>DAT_CORRECAO</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>DEBITO_20180115</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>TIP_ORIGEM_SISTEMA</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>DEBITO_20180115</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>VLR_PRINCIPAL_ORIGINAL</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>DEBITO_20180115</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>VLR_MULTA_ORIGINAL</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>DEBITO_20180115</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>DAT_INCLUSAO</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>DEBITO_20180115</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>NUM_MES_REFERENCIA</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>DEBITO_20180115</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>NUM_ANO_REFERENCIA</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>DEBITO_20180115</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>STA_DEBITO</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>DEBITO_20180115</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>NUM_VERSAO</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_ATUAL</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>SEQ_LANCAMENTO</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_ATUAL</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>SEQ_DEBITO</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_ATUAL</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>SEQ_TIPO_LANCAMENTO</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_ATUAL</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>SEQ_DOCUMENTO_CREDITO</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_ATUAL</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>COD_RECEITA</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_ATUAL</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>SEQ_PESSOA</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_ATUAL</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>DAT_LANCAMENTO</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_ATUAL</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>DAT_VENCIMENTO</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_ATUAL</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>NUM_MES_REFERENCIA</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_ATUAL</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>NUM_ANO_REFERENCIA</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_ATUAL</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>VLR_LANCAMENTO</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_ATUAL</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>DSC_INFORM_COMPLEMENT</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_ATUAL</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>NUM_VERSAO</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_TMP</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>SEQ_LANCAMENTO</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_TMP</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>SEQ_DEBITO</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_TMP</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>SEQ_TIPO_LANCAMENTO</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_TMP</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>SEQ_DOCUMENTO_CREDITO</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_TMP</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>COD_RECEITA</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_TMP</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>SEQ_PESSOA</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_TMP</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>DAT_LANCAMENTO</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_TMP</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>DAT_VENCIMENTO</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr"/>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_TMP</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>NUM_MES_REFERENCIA</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_TMP</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>NUM_ANO_REFERENCIA</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_TMP</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>VLR_LANCAMENTO</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_TMP</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>DSC_INFORM_COMPLEMENT</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_TMP</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>NUM_VERSAO</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_20180115</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>SEQ_LANCAMENTO</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_20180115</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>SEQ_DEBITO</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_20180115</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>SEQ_TIPO_LANCAMENTO</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr"/>
-      <c r="G47" t="inlineStr"/>
-      <c r="H47" t="inlineStr"/>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_20180115</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>SEQ_DOCUMENTO_CREDITO</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr"/>
-      <c r="G48" t="inlineStr"/>
-      <c r="H48" t="inlineStr"/>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_20180115</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>COD_RECEITA</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr"/>
-      <c r="H49" t="inlineStr"/>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_20180115</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>SEQ_PESSOA</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr"/>
-      <c r="H50" t="inlineStr"/>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_20180115</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>DAT_LANCAMENTO</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr"/>
-      <c r="H51" t="inlineStr"/>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_20180115</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>DAT_VENCIMENTO</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr"/>
-      <c r="H52" t="inlineStr"/>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_20180115</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>NUM_MES_REFERENCIA</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr"/>
-      <c r="G53" t="inlineStr"/>
-      <c r="H53" t="inlineStr"/>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_20180115</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>NUM_ANO_REFERENCIA</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr"/>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="inlineStr"/>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_20180115</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>VLR_LANCAMENTO</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr"/>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="inlineStr"/>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_20180115</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>DSC_INFORM_COMPLEMENT</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr"/>
-      <c r="G56" t="inlineStr"/>
-      <c r="H56" t="inlineStr"/>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>MQMD10</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Total number of tables with column names without comments</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>LANCAMENTO_20180115</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>NUM_VERSAO</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr"/>
-      <c r="G57" t="inlineStr"/>
-      <c r="H57" t="inlineStr"/>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>MQMD12</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>Total number of tables with non-standard foreign key prefixes</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>CONTA_CORRENTE</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>LANCAMENTO</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>SEQ_TIPO_LANCAMENTO</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>SYS_C001517488</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr"/>
-      <c r="H58" t="inlineStr"/>
+          <t>Total number of unique key</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15790,7 +14130,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15801,94 +14141,1754 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Indicator</t>
+          <t>rule</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>desc</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Value</t>
+          <t>owner</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>table</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>column</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>constraint_name</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>length</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>limit</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MQMD01</t>
+          <t>MQME10</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Total number of tables</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>21</v>
-      </c>
+          <t>Total number of tables with plural names</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>AUDITORIA_ENTIDADES</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MQMD02</t>
+          <t>MQME01</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Total number of columns</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>217</v>
-      </c>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>DEBITO_20180115</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>SEQ_DEBITO</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MQMD03</t>
+          <t>MQME01</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Total number of primary key</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>20</v>
-      </c>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>DEBITO_20180115</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>SEQ_DEBITO_ORIGEM</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MQMD04</t>
+          <t>MQME01</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Total number of foreign key</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>24</v>
-      </c>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>DEBITO_20180115</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>COD_RECEITA</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MQMD05</t>
+          <t>MQME01</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Total number of unique key</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>DEBITO_20180115</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>COD_INDICADOR</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>DEBITO_20180115</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>COD_PRODUTO_SERVICO</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>DEBITO_20180115</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>SEQ_PESSOA</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>DEBITO_20180115</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>DAT_VENCIMENTO</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>DEBITO_20180115</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>DAT_CORRECAO</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>DEBITO_20180115</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>TIP_ORIGEM_SISTEMA</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>DEBITO_20180115</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>VLR_PRINCIPAL_ORIGINAL</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>DEBITO_20180115</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>VLR_MULTA_ORIGINAL</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>DEBITO_20180115</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>DAT_INCLUSAO</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>DEBITO_20180115</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>NUM_MES_REFERENCIA</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>DEBITO_20180115</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>NUM_ANO_REFERENCIA</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>DEBITO_20180115</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>STA_DEBITO</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>DEBITO_20180115</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>NUM_VERSAO</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_ATUAL</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>SEQ_LANCAMENTO</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_ATUAL</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>SEQ_DEBITO</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_ATUAL</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>SEQ_TIPO_LANCAMENTO</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_ATUAL</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>SEQ_DOCUMENTO_CREDITO</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_ATUAL</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>COD_RECEITA</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_ATUAL</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>SEQ_PESSOA</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_ATUAL</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>DAT_LANCAMENTO</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_ATUAL</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>DAT_VENCIMENTO</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_ATUAL</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>NUM_MES_REFERENCIA</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_ATUAL</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>NUM_ANO_REFERENCIA</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_ATUAL</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>VLR_LANCAMENTO</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_ATUAL</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>DSC_INFORM_COMPLEMENT</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_ATUAL</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>NUM_VERSAO</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_TMP</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>SEQ_LANCAMENTO</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_TMP</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>SEQ_DEBITO</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_TMP</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>SEQ_TIPO_LANCAMENTO</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_TMP</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>SEQ_DOCUMENTO_CREDITO</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_TMP</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>COD_RECEITA</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_TMP</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>SEQ_PESSOA</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_TMP</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>DAT_LANCAMENTO</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_TMP</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>DAT_VENCIMENTO</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_TMP</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>NUM_MES_REFERENCIA</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_TMP</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>NUM_ANO_REFERENCIA</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_TMP</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>VLR_LANCAMENTO</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_TMP</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>DSC_INFORM_COMPLEMENT</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_TMP</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>NUM_VERSAO</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_20180115</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>SEQ_LANCAMENTO</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_20180115</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>SEQ_DEBITO</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_20180115</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>SEQ_TIPO_LANCAMENTO</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_20180115</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>SEQ_DOCUMENTO_CREDITO</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_20180115</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>COD_RECEITA</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_20180115</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>SEQ_PESSOA</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_20180115</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>DAT_LANCAMENTO</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_20180115</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>DAT_VENCIMENTO</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_20180115</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>NUM_MES_REFERENCIA</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_20180115</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>NUM_ANO_REFERENCIA</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_20180115</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>VLR_LANCAMENTO</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_20180115</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>DSC_INFORM_COMPLEMENT</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>MQME01</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Columns without comments</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>LANCAMENTO_20180115</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>NUM_VERSAO</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>MQME15</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Total number of tables with non-standard foreign key prefixes</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>CONTA_CORRENTE</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>LANCAMENTO</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>SEQ_TIPO_LANCAMENTO</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>SYS_C001517488</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15929,46 +15929,46 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MQMD06</t>
+          <t>MQME00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Total number of tables with plural names</t>
+          <t>Total number of columns</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MQMD10</t>
+          <t>MQMEA1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Total number of tables with column names without comments</t>
+          <t>Total number of length-required columns</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>55</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MQMD12</t>
+          <t>MQMEA2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Total number of tables with non-standard foreign key prefixes</t>
+          <t>Total number of NUMBER columns</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -15982,7 +15982,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16010,29 +16010,29 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IQMD01</t>
+          <t>IQME01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Table names in singular</t>
+          <t>Columns with comments</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>95.24%</t>
+          <t>74.65%</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IQMD02</t>
+          <t>IQME02</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Table names with recommended size</t>
+          <t>Columns with data type</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -16044,12 +16044,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>IQMD03</t>
+          <t>IQME03</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Table columns with correct prefixes</t>
+          <t>Length-required columns with data length</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -16061,12 +16061,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>IQMD04</t>
+          <t>IQME04</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Table columns with recommend size</t>
+          <t>NUMBER columns with valid scale</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -16078,29 +16078,29 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IQMD05</t>
+          <t>IQME05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Table columns with comments</t>
+          <t>Columns with valid num_distinct</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>74.65%</t>
+          <t>100.00%</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>IQMD06</t>
+          <t>IQME06</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Table with standard PK prefixes</t>
+          <t>Columns with valid num_nulls</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -16112,34 +16112,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>IQMD07</t>
+          <t>IQME07</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Table with standard FK prefixes</t>
+          <t>Columns with valid density</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>95.83%</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>IQMD08</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Table with standard UK prefixes</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>0.00%</t>
+          <t>100.00%</t>
         </is>
       </c>
     </row>

</xml_diff>